<commit_message>
Reorganizing test default models and unit models, refactoring test methods.
</commit_message>
<xml_diff>
--- a/default/3_sut_multi_year_rcot_cap/sets.xlsx
+++ b/default/3_sut_multi_year_rcot_cap/sets.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\3_sut_multi_year_rcot_cap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\3_sut_multi_year_rcot_cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F056259-38AE-4FE0-974C-E47838D276B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C23CAD3-5BC0-4B79-959D-35A5B2C33C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57510" yWindow="0" windowWidth="19380" windowHeight="20970" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23290" yWindow="3420" windowWidth="21200" windowHeight="15370" tabRatio="943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_SCENARIOS" sheetId="1" r:id="rId1"/>
-    <sheet name="_set_SUP_TECH" sheetId="2" r:id="rId2"/>
-    <sheet name="_set_DEM_TECH" sheetId="3" r:id="rId3"/>
+    <sheet name="_set_TECH_SUP" sheetId="2" r:id="rId2"/>
+    <sheet name="_set_TECH_DEM" sheetId="3" r:id="rId3"/>
     <sheet name="_set_FLOWS" sheetId="4" r:id="rId4"/>
     <sheet name="_set_FLOWS_AGG" sheetId="5" r:id="rId5"/>
-    <sheet name="_set_YEARS" sheetId="6" r:id="rId6"/>
+    <sheet name="_set_COSTS" sheetId="6" r:id="rId6"/>
+    <sheet name="_set_EMISSIONS" sheetId="7" r:id="rId7"/>
+    <sheet name="_set_LOADFACTORS" sheetId="8" r:id="rId8"/>
+    <sheet name="_set_YEARS" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>s_Name</t>
   </si>
@@ -39,13 +42,22 @@
     <t>f_Name</t>
   </si>
   <si>
-    <t>f_Name_agg</t>
-  </si>
-  <si>
-    <t>f_Unit</t>
-  </si>
-  <si>
-    <t>fa_Name</t>
+    <t>f_agg_Name</t>
+  </si>
+  <si>
+    <t>c_Name</t>
+  </si>
+  <si>
+    <t>c_Category</t>
+  </si>
+  <si>
+    <t>e_Name</t>
+  </si>
+  <si>
+    <t>lf_Name</t>
+  </si>
+  <si>
+    <t>lf_Category</t>
   </si>
   <si>
     <t>y_Name</t>
@@ -63,25 +75,40 @@
     <t>Transport</t>
   </si>
   <si>
-    <t>Final demand</t>
+    <t>households</t>
   </si>
   <si>
     <t>Electricity from Fossil</t>
   </si>
   <si>
+    <t>Electricity</t>
+  </si>
+  <si>
     <t>Electricity from non-Fossil</t>
   </si>
   <si>
     <t>Transport service</t>
   </si>
   <si>
-    <t>Electricity</t>
-  </si>
-  <si>
-    <t>TWh</t>
-  </si>
-  <si>
-    <t>Mkm</t>
+    <t>Capital costs</t>
+  </si>
+  <si>
+    <t>Operational costs</t>
+  </si>
+  <si>
+    <t>CO2 emissions</t>
+  </si>
+  <si>
+    <t>lf max</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>lf min</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
   <si>
     <t>y1</t>
@@ -461,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,7 +501,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +514,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,17 +526,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +549,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,7 +561,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -544,56 +571,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <selection activeCell="A2" sqref="A2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -613,17 +628,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -633,42 +648,145 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>